<commit_message>
Fixed the NaNs in Skaters
</commit_message>
<xml_diff>
--- a/DataCleaning/Instat_DataCleaning/SkatersCleaned.xlsx
+++ b/DataCleaning/Instat_DataCleaning/SkatersCleaned.xlsx
@@ -1896,7 +1896,9 @@
       <c r="BN3" t="n">
         <v>1.03</v>
       </c>
-      <c r="BO3" t="inlineStr"/>
+      <c r="BO3" t="n">
+        <v>0</v>
+      </c>
       <c r="BP3" t="n">
         <v>-7</v>
       </c>
@@ -5718,7 +5720,9 @@
       <c r="BN11" t="n">
         <v>0.92</v>
       </c>
-      <c r="BO11" t="inlineStr"/>
+      <c r="BO11" t="n">
+        <v>0</v>
+      </c>
       <c r="BP11" t="n">
         <v>-8</v>
       </c>
@@ -6194,7 +6198,9 @@
       <c r="BN12" t="n">
         <v>1</v>
       </c>
-      <c r="BO12" t="inlineStr"/>
+      <c r="BO12" t="n">
+        <v>0</v>
+      </c>
       <c r="BP12" t="n">
         <v>-5.2</v>
       </c>
@@ -7148,7 +7154,9 @@
       <c r="BN14" t="n">
         <v>0.73</v>
       </c>
-      <c r="BO14" t="inlineStr"/>
+      <c r="BO14" t="n">
+        <v>0</v>
+      </c>
       <c r="BP14" t="n">
         <v>-8</v>
       </c>
@@ -7624,7 +7632,9 @@
       <c r="BN15" t="n">
         <v>0.44</v>
       </c>
-      <c r="BO15" t="inlineStr"/>
+      <c r="BO15" t="n">
+        <v>0</v>
+      </c>
       <c r="BP15" t="n">
         <v>-3.5</v>
       </c>
@@ -8578,7 +8588,9 @@
       <c r="BN17" t="n">
         <v>1.56</v>
       </c>
-      <c r="BO17" t="inlineStr"/>
+      <c r="BO17" t="n">
+        <v>0</v>
+      </c>
       <c r="BP17" t="n">
         <v>-11</v>
       </c>
@@ -9532,7 +9544,9 @@
       <c r="BN19" t="n">
         <v>0.66</v>
       </c>
-      <c r="BO19" t="inlineStr"/>
+      <c r="BO19" t="n">
+        <v>0</v>
+      </c>
       <c r="BP19" t="n">
         <v>-3.8</v>
       </c>
@@ -10008,7 +10022,9 @@
       <c r="BN20" t="n">
         <v>0.6</v>
       </c>
-      <c r="BO20" t="inlineStr"/>
+      <c r="BO20" t="n">
+        <v>0</v>
+      </c>
       <c r="BP20" t="n">
         <v>-2.7</v>
       </c>
@@ -10484,7 +10500,9 @@
       <c r="BN21" t="n">
         <v>0.57</v>
       </c>
-      <c r="BO21" t="inlineStr"/>
+      <c r="BO21" t="n">
+        <v>0</v>
+      </c>
       <c r="BP21" t="n">
         <v>-4.8</v>
       </c>
@@ -10960,7 +10978,9 @@
       <c r="BN22" t="n">
         <v>0.3</v>
       </c>
-      <c r="BO22" t="inlineStr"/>
+      <c r="BO22" t="n">
+        <v>0</v>
+      </c>
       <c r="BP22" t="n">
         <v>0</v>
       </c>
@@ -11436,7 +11456,9 @@
       <c r="BN23" t="n">
         <v>0.08</v>
       </c>
-      <c r="BO23" t="inlineStr"/>
+      <c r="BO23" t="n">
+        <v>0</v>
+      </c>
       <c r="BP23" t="n">
         <v>0</v>
       </c>
@@ -12390,7 +12412,9 @@
       <c r="BN25" t="n">
         <v>0.25</v>
       </c>
-      <c r="BO25" t="inlineStr"/>
+      <c r="BO25" t="n">
+        <v>0</v>
+      </c>
       <c r="BP25" t="n">
         <v>0</v>
       </c>
@@ -12866,7 +12890,9 @@
       <c r="BN26" t="n">
         <v>0.01</v>
       </c>
-      <c r="BO26" t="inlineStr"/>
+      <c r="BO26" t="n">
+        <v>0</v>
+      </c>
       <c r="BP26" t="n">
         <v>0</v>
       </c>
@@ -13342,7 +13368,9 @@
       <c r="BN27" t="n">
         <v>0.14</v>
       </c>
-      <c r="BO27" t="inlineStr"/>
+      <c r="BO27" t="n">
+        <v>0</v>
+      </c>
       <c r="BP27" t="n">
         <v>0</v>
       </c>
@@ -13818,7 +13846,9 @@
       <c r="BN28" t="n">
         <v>0.23</v>
       </c>
-      <c r="BO28" t="inlineStr"/>
+      <c r="BO28" t="n">
+        <v>0</v>
+      </c>
       <c r="BP28" t="n">
         <v>0</v>
       </c>
@@ -14294,7 +14324,9 @@
       <c r="BN29" t="n">
         <v>0.18</v>
       </c>
-      <c r="BO29" t="inlineStr"/>
+      <c r="BO29" t="n">
+        <v>0</v>
+      </c>
       <c r="BP29" t="n">
         <v>0</v>
       </c>
@@ -14770,7 +14802,9 @@
       <c r="BN30" t="n">
         <v>0.3</v>
       </c>
-      <c r="BO30" t="inlineStr"/>
+      <c r="BO30" t="n">
+        <v>0</v>
+      </c>
       <c r="BP30" t="n">
         <v>0</v>
       </c>
@@ -15246,7 +15280,9 @@
       <c r="BN31" t="n">
         <v>0.25</v>
       </c>
-      <c r="BO31" t="inlineStr"/>
+      <c r="BO31" t="n">
+        <v>0</v>
+      </c>
       <c r="BP31" t="n">
         <v>0</v>
       </c>
@@ -15722,7 +15758,9 @@
       <c r="BN32" t="n">
         <v>0.01</v>
       </c>
-      <c r="BO32" t="inlineStr"/>
+      <c r="BO32" t="n">
+        <v>0</v>
+      </c>
       <c r="BP32" t="n">
         <v>0</v>
       </c>
@@ -16198,7 +16236,9 @@
       <c r="BN33" t="n">
         <v>0.04</v>
       </c>
-      <c r="BO33" t="inlineStr"/>
+      <c r="BO33" t="n">
+        <v>0</v>
+      </c>
       <c r="BP33" t="n">
         <v>0</v>
       </c>
@@ -16674,7 +16714,9 @@
       <c r="BN34" t="n">
         <v>0.02</v>
       </c>
-      <c r="BO34" t="inlineStr"/>
+      <c r="BO34" t="n">
+        <v>0</v>
+      </c>
       <c r="BP34" t="n">
         <v>0</v>
       </c>
@@ -17150,7 +17192,9 @@
       <c r="BN35" t="n">
         <v>0</v>
       </c>
-      <c r="BO35" t="inlineStr"/>
+      <c r="BO35" t="n">
+        <v>0</v>
+      </c>
       <c r="BP35" t="n">
         <v>0</v>
       </c>
@@ -17626,7 +17670,9 @@
       <c r="BN36" t="n">
         <v>0.33</v>
       </c>
-      <c r="BO36" t="inlineStr"/>
+      <c r="BO36" t="n">
+        <v>0</v>
+      </c>
       <c r="BP36" t="n">
         <v>0</v>
       </c>
@@ -18102,7 +18148,9 @@
       <c r="BN37" t="n">
         <v>0.51</v>
       </c>
-      <c r="BO37" t="inlineStr"/>
+      <c r="BO37" t="n">
+        <v>0</v>
+      </c>
       <c r="BP37" t="n">
         <v>0</v>
       </c>
@@ -18578,7 +18626,9 @@
       <c r="BN38" t="n">
         <v>0.51</v>
       </c>
-      <c r="BO38" t="inlineStr"/>
+      <c r="BO38" t="n">
+        <v>0</v>
+      </c>
       <c r="BP38" t="n">
         <v>0</v>
       </c>
@@ -19054,7 +19104,9 @@
       <c r="BN39" t="n">
         <v>0.22</v>
       </c>
-      <c r="BO39" t="inlineStr"/>
+      <c r="BO39" t="n">
+        <v>0</v>
+      </c>
       <c r="BP39" t="n">
         <v>0</v>
       </c>
@@ -19530,7 +19582,9 @@
       <c r="BN40" t="n">
         <v>0</v>
       </c>
-      <c r="BO40" t="inlineStr"/>
+      <c r="BO40" t="n">
+        <v>0</v>
+      </c>
       <c r="BP40" t="n">
         <v>0</v>
       </c>
@@ -20006,7 +20060,9 @@
       <c r="BN41" t="n">
         <v>0.03</v>
       </c>
-      <c r="BO41" t="inlineStr"/>
+      <c r="BO41" t="n">
+        <v>0</v>
+      </c>
       <c r="BP41" t="n">
         <v>0</v>
       </c>
@@ -20482,7 +20538,9 @@
       <c r="BN42" t="n">
         <v>0.03</v>
       </c>
-      <c r="BO42" t="inlineStr"/>
+      <c r="BO42" t="n">
+        <v>0</v>
+      </c>
       <c r="BP42" t="n">
         <v>0</v>
       </c>
@@ -20958,7 +21016,9 @@
       <c r="BN43" t="n">
         <v>0.06</v>
       </c>
-      <c r="BO43" t="inlineStr"/>
+      <c r="BO43" t="n">
+        <v>0</v>
+      </c>
       <c r="BP43" t="n">
         <v>0</v>
       </c>
@@ -21434,7 +21494,9 @@
       <c r="BN44" t="n">
         <v>0</v>
       </c>
-      <c r="BO44" t="inlineStr"/>
+      <c r="BO44" t="n">
+        <v>0</v>
+      </c>
       <c r="BP44" t="n">
         <v>0</v>
       </c>
@@ -21910,7 +21972,9 @@
       <c r="BN45" t="n">
         <v>0</v>
       </c>
-      <c r="BO45" t="inlineStr"/>
+      <c r="BO45" t="n">
+        <v>0</v>
+      </c>
       <c r="BP45" t="n">
         <v>0</v>
       </c>
@@ -22386,7 +22450,9 @@
       <c r="BN46" t="n">
         <v>0.01</v>
       </c>
-      <c r="BO46" t="inlineStr"/>
+      <c r="BO46" t="n">
+        <v>0</v>
+      </c>
       <c r="BP46" t="n">
         <v>0</v>
       </c>
@@ -22862,7 +22928,9 @@
       <c r="BN47" t="n">
         <v>0.07000000000000001</v>
       </c>
-      <c r="BO47" t="inlineStr"/>
+      <c r="BO47" t="n">
+        <v>0</v>
+      </c>
       <c r="BP47" t="n">
         <v>0</v>
       </c>
@@ -23338,7 +23406,9 @@
       <c r="BN48" t="n">
         <v>0.05</v>
       </c>
-      <c r="BO48" t="inlineStr"/>
+      <c r="BO48" t="n">
+        <v>0</v>
+      </c>
       <c r="BP48" t="n">
         <v>0</v>
       </c>
@@ -23814,7 +23884,9 @@
       <c r="BN49" t="n">
         <v>0.02</v>
       </c>
-      <c r="BO49" t="inlineStr"/>
+      <c r="BO49" t="n">
+        <v>0</v>
+      </c>
       <c r="BP49" t="n">
         <v>0</v>
       </c>
@@ -24290,7 +24362,9 @@
       <c r="BN50" t="n">
         <v>0.04</v>
       </c>
-      <c r="BO50" t="inlineStr"/>
+      <c r="BO50" t="n">
+        <v>0</v>
+      </c>
       <c r="BP50" t="n">
         <v>0</v>
       </c>
@@ -24766,7 +24840,9 @@
       <c r="BN51" t="n">
         <v>0.05</v>
       </c>
-      <c r="BO51" t="inlineStr"/>
+      <c r="BO51" t="n">
+        <v>0</v>
+      </c>
       <c r="BP51" t="n">
         <v>0</v>
       </c>
@@ -25242,7 +25318,9 @@
       <c r="BN52" t="n">
         <v>0.08</v>
       </c>
-      <c r="BO52" t="inlineStr"/>
+      <c r="BO52" t="n">
+        <v>0</v>
+      </c>
       <c r="BP52" t="n">
         <v>0</v>
       </c>
@@ -25718,7 +25796,9 @@
       <c r="BN53" t="n">
         <v>0.06</v>
       </c>
-      <c r="BO53" t="inlineStr"/>
+      <c r="BO53" t="n">
+        <v>0</v>
+      </c>
       <c r="BP53" t="n">
         <v>0</v>
       </c>
@@ -26194,7 +26274,9 @@
       <c r="BN54" t="n">
         <v>0</v>
       </c>
-      <c r="BO54" t="inlineStr"/>
+      <c r="BO54" t="n">
+        <v>0</v>
+      </c>
       <c r="BP54" t="n">
         <v>0</v>
       </c>
@@ -26670,7 +26752,9 @@
       <c r="BN55" t="n">
         <v>0.01</v>
       </c>
-      <c r="BO55" t="inlineStr"/>
+      <c r="BO55" t="n">
+        <v>0</v>
+      </c>
       <c r="BP55" t="n">
         <v>0</v>
       </c>
@@ -28102,7 +28186,9 @@
       <c r="BN58" t="n">
         <v>0.06</v>
       </c>
-      <c r="BO58" t="inlineStr"/>
+      <c r="BO58" t="n">
+        <v>0</v>
+      </c>
       <c r="BP58" t="n">
         <v>0</v>
       </c>
@@ -28578,7 +28664,9 @@
       <c r="BN59" t="n">
         <v>0</v>
       </c>
-      <c r="BO59" t="inlineStr"/>
+      <c r="BO59" t="n">
+        <v>0</v>
+      </c>
       <c r="BP59" t="n">
         <v>0</v>
       </c>
@@ -29054,7 +29142,9 @@
       <c r="BN60" t="n">
         <v>0.03</v>
       </c>
-      <c r="BO60" t="inlineStr"/>
+      <c r="BO60" t="n">
+        <v>0</v>
+      </c>
       <c r="BP60" t="n">
         <v>0</v>
       </c>
@@ -29530,7 +29620,9 @@
       <c r="BN61" t="n">
         <v>0.01</v>
       </c>
-      <c r="BO61" t="inlineStr"/>
+      <c r="BO61" t="n">
+        <v>0</v>
+      </c>
       <c r="BP61" t="n">
         <v>0</v>
       </c>
@@ -30484,7 +30576,9 @@
       <c r="BN63" t="n">
         <v>1.17</v>
       </c>
-      <c r="BO63" t="inlineStr"/>
+      <c r="BO63" t="n">
+        <v>0</v>
+      </c>
       <c r="BP63" t="n">
         <v>-7</v>
       </c>
@@ -34306,7 +34400,9 @@
       <c r="BN71" t="n">
         <v>1.22</v>
       </c>
-      <c r="BO71" t="inlineStr"/>
+      <c r="BO71" t="n">
+        <v>0</v>
+      </c>
       <c r="BP71" t="n">
         <v>-8</v>
       </c>
@@ -34782,7 +34878,9 @@
       <c r="BN72" t="n">
         <v>1.09</v>
       </c>
-      <c r="BO72" t="inlineStr"/>
+      <c r="BO72" t="n">
+        <v>0</v>
+      </c>
       <c r="BP72" t="n">
         <v>-5.2</v>
       </c>
@@ -35736,7 +35834,9 @@
       <c r="BN74" t="n">
         <v>0.75</v>
       </c>
-      <c r="BO74" t="inlineStr"/>
+      <c r="BO74" t="n">
+        <v>0</v>
+      </c>
       <c r="BP74" t="n">
         <v>-8</v>
       </c>
@@ -36212,7 +36312,9 @@
       <c r="BN75" t="n">
         <v>0.45</v>
       </c>
-      <c r="BO75" t="inlineStr"/>
+      <c r="BO75" t="n">
+        <v>0</v>
+      </c>
       <c r="BP75" t="n">
         <v>-3.5</v>
       </c>
@@ -38122,7 +38224,9 @@
       <c r="BN79" t="n">
         <v>0.88</v>
       </c>
-      <c r="BO79" t="inlineStr"/>
+      <c r="BO79" t="n">
+        <v>0</v>
+      </c>
       <c r="BP79" t="n">
         <v>-3.8</v>
       </c>
@@ -38598,7 +38702,9 @@
       <c r="BN80" t="n">
         <v>0.64</v>
       </c>
-      <c r="BO80" t="inlineStr"/>
+      <c r="BO80" t="n">
+        <v>0</v>
+      </c>
       <c r="BP80" t="n">
         <v>-2.7</v>
       </c>
@@ -39074,7 +39180,9 @@
       <c r="BN81" t="n">
         <v>0.62</v>
       </c>
-      <c r="BO81" t="inlineStr"/>
+      <c r="BO81" t="n">
+        <v>0</v>
+      </c>
       <c r="BP81" t="n">
         <v>-4.8</v>
       </c>

</xml_diff>

<commit_message>
Updated column names to match database
</commit_message>
<xml_diff>
--- a/DataCleaning/Instat_DataCleaning/SkatersCleaned.xlsx
+++ b/DataCleaning/Instat_DataCleaning/SkatersCleaned.xlsx
@@ -1116,102 +1116,102 @@
       </c>
       <c r="EG1" s="1" t="inlineStr">
         <is>
-          <t>Time on ice_minutes</t>
+          <t>Time on ice (Minutes)</t>
         </is>
       </c>
       <c r="EH1" s="1" t="inlineStr">
         <is>
-          <t>Time on ice_seconds</t>
+          <t>Time on ice (Seconds)</t>
         </is>
       </c>
       <c r="EI1" s="1" t="inlineStr">
         <is>
-          <t>Penalty time_minutes</t>
+          <t>Penalty time (Minutes)</t>
         </is>
       </c>
       <c r="EJ1" s="1" t="inlineStr">
         <is>
-          <t>Penalty time_seconds</t>
+          <t>Penalty time (Seconds)</t>
         </is>
       </c>
       <c r="EK1" s="1" t="inlineStr">
         <is>
-          <t>Puck control time_minutes</t>
+          <t>Puck control time (Minutes)</t>
         </is>
       </c>
       <c r="EL1" s="1" t="inlineStr">
         <is>
-          <t>Puck control time_seconds</t>
+          <t>Puck control time (Seconds)</t>
         </is>
       </c>
       <c r="EM1" s="1" t="inlineStr">
         <is>
-          <t>Power play time_minutes</t>
+          <t>Power play time (Minutes)</t>
         </is>
       </c>
       <c r="EN1" s="1" t="inlineStr">
         <is>
-          <t>Power play time_seconds</t>
+          <t>Power play time (Seconds)</t>
         </is>
       </c>
       <c r="EO1" s="1" t="inlineStr">
         <is>
-          <t>Short-handed time_minutes</t>
+          <t>Short-handed time (Minutes)</t>
         </is>
       </c>
       <c r="EP1" s="1" t="inlineStr">
         <is>
-          <t>Short-handed time_seconds</t>
+          <t>Short-handed time (Seconds)</t>
         </is>
       </c>
       <c r="EQ1" s="1" t="inlineStr">
         <is>
-          <t>Playing in attack_minutes</t>
+          <t>Playing in attack (Minutes)</t>
         </is>
       </c>
       <c r="ER1" s="1" t="inlineStr">
         <is>
-          <t>Playing in attack_seconds</t>
+          <t>Playing in attack (Seconds)</t>
         </is>
       </c>
       <c r="ES1" s="1" t="inlineStr">
         <is>
-          <t>Playing in defense_minutes</t>
+          <t>Playing in defense (Minutes)</t>
         </is>
       </c>
       <c r="ET1" s="1" t="inlineStr">
         <is>
-          <t>Playing in defense_seconds</t>
+          <t>Playing in defense (Seconds)</t>
         </is>
       </c>
       <c r="EU1" s="1" t="inlineStr">
         <is>
-          <t>OZ possession_minutes</t>
+          <t>OZ possession (Minutes)</t>
         </is>
       </c>
       <c r="EV1" s="1" t="inlineStr">
         <is>
-          <t>OZ possession_seconds</t>
+          <t>OZ possession (Seconds)</t>
         </is>
       </c>
       <c r="EW1" s="1" t="inlineStr">
         <is>
-          <t>NZ possession_minutes</t>
+          <t>NZ possession (Minutes)</t>
         </is>
       </c>
       <c r="EX1" s="1" t="inlineStr">
         <is>
-          <t>NZ possession_seconds</t>
+          <t>NZ possession (Seconds)</t>
         </is>
       </c>
       <c r="EY1" s="1" t="inlineStr">
         <is>
-          <t>DZ possession_minutes</t>
+          <t>DZ possession (Minutes)</t>
         </is>
       </c>
       <c r="EZ1" s="1" t="inlineStr">
         <is>
-          <t>DZ possession_seconds</t>
+          <t>DZ possession (Seconds)</t>
         </is>
       </c>
     </row>

</xml_diff>